<commit_message>
fee updated by the xls file
</commit_message>
<xml_diff>
--- a/static/classes/classes.xlsx
+++ b/static/classes/classes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/david/Documents/Development/django-bmx/static/classes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{123744BA-C57B-EB48-AACC-8CF4E4912E54}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0D18A39-88C1-1F41-83D1-02B3F5196140}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="57">
   <si>
     <t xml:space="preserve">Girls bonus </t>
   </si>
@@ -185,6 +185,21 @@
   </si>
   <si>
     <t>Boys 15 and 16</t>
+  </si>
+  <si>
+    <t>fee</t>
+  </si>
+  <si>
+    <t>MČR</t>
+  </si>
+  <si>
+    <t>Český pohár</t>
+  </si>
+  <si>
+    <t>Česká a Moravská liga</t>
+  </si>
+  <si>
+    <t>Volný</t>
   </si>
 </sst>
 </file>
@@ -198,16 +213,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="12"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
       <sz val="14"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -216,6 +221,18 @@
       <sz val="14"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="238"/>
     </font>
   </fonts>
   <fills count="2">
@@ -238,7 +255,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -251,23 +268,26 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
@@ -582,255 +602,663 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AMJ35"/>
+  <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.33203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="17.6640625" style="1" customWidth="1"/>
-    <col min="3" max="4" width="11.5" style="1"/>
-    <col min="5" max="5" width="8.5" style="1" customWidth="1"/>
-    <col min="6" max="6" width="20.33203125" style="1" customWidth="1"/>
-    <col min="7" max="1024" width="11.5" style="1"/>
+    <col min="1" max="1" width="29.5" style="10" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" style="10" customWidth="1"/>
+    <col min="3" max="3" width="15.1640625" style="10" customWidth="1"/>
+    <col min="4" max="4" width="11.5" style="10"/>
+    <col min="5" max="5" width="8.5" style="10" customWidth="1"/>
+    <col min="6" max="6" width="20.33203125" style="10" customWidth="1"/>
+    <col min="7" max="16384" width="11.5" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="2"/>
-      <c r="B1" s="11" t="s">
+    <row r="1" spans="1:8" ht="19" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="11"/>
-    </row>
-    <row r="2" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="4"/>
-      <c r="B2" s="3" t="s">
+      <c r="C1" s="9"/>
+      <c r="D1" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="11"/>
+      <c r="B2" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="12" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:8" ht="19" x14ac:dyDescent="0.2">
+      <c r="A3" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="D3" s="10">
+        <v>400</v>
+      </c>
+      <c r="E3" s="10">
+        <v>400</v>
+      </c>
+      <c r="F3" s="8" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+      <c r="G3" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="H3" s="10">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="19" x14ac:dyDescent="0.2">
+      <c r="A4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="D4" s="10">
+        <v>400</v>
+      </c>
+      <c r="E4" s="10">
+        <v>400</v>
+      </c>
+      <c r="F4" s="8" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
+      <c r="G4" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="H4" s="10">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="19" x14ac:dyDescent="0.2">
+      <c r="A5" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="D5" s="10">
+        <v>400</v>
+      </c>
+      <c r="E5" s="10">
+        <v>400</v>
+      </c>
+      <c r="F5" s="8" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+      <c r="G5" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="H5" s="10">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="19" x14ac:dyDescent="0.2">
+      <c r="A6" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="D6" s="10">
+        <v>400</v>
+      </c>
+      <c r="E6" s="10">
+        <v>400</v>
+      </c>
+      <c r="F6" s="8" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
+      <c r="G6" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="H6" s="10">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="19" x14ac:dyDescent="0.2">
+      <c r="A7" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="B7" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="10">
+        <v>400</v>
+      </c>
+      <c r="E7" s="10">
+        <v>400</v>
+      </c>
+      <c r="F7" s="8" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
+      <c r="G7" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="H7" s="10">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="19" x14ac:dyDescent="0.2">
+      <c r="A8" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="B8" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="10">
+        <v>400</v>
+      </c>
+      <c r="E8" s="10">
+        <v>400</v>
+      </c>
+      <c r="F8" s="8" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
+      <c r="G8" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="H8" s="10">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="19" x14ac:dyDescent="0.2">
+      <c r="A9" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="B9" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="10">
+        <v>400</v>
+      </c>
+      <c r="E9" s="10">
+        <v>400</v>
+      </c>
+      <c r="F9" s="8" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
+      <c r="G9" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="H9" s="10">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="19" x14ac:dyDescent="0.2">
+      <c r="A10" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="B10" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="D10" s="10">
+        <v>400</v>
+      </c>
+      <c r="E10" s="10">
+        <v>400</v>
+      </c>
+      <c r="F10" s="8" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
+      <c r="G10" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="H10" s="10">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="19" x14ac:dyDescent="0.2">
+      <c r="A11" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="B11" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="D11" s="10">
+        <v>400</v>
+      </c>
+      <c r="E11" s="10">
+        <v>400</v>
+      </c>
+      <c r="F11" s="8" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
+      <c r="G11" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="H11" s="10">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="B12" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="D12" s="10">
+        <v>400</v>
+      </c>
+      <c r="E12" s="10">
+        <v>400</v>
+      </c>
+      <c r="F12" s="8" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
+      <c r="G12" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="H12" s="10">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="19" x14ac:dyDescent="0.2">
+      <c r="A13" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="B13" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="D13" s="10">
+        <v>400</v>
+      </c>
+      <c r="E13" s="10">
+        <v>400</v>
+      </c>
+      <c r="F13" s="8" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
+      <c r="G13" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="H13" s="10">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="19" x14ac:dyDescent="0.2">
+      <c r="A14" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="B14" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D14" s="10">
+        <v>400</v>
+      </c>
+      <c r="E14" s="10">
+        <v>400</v>
+      </c>
+      <c r="F14" s="8" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
+      <c r="G14" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="H14" s="10">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="19" x14ac:dyDescent="0.2">
+      <c r="A15" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="B15" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D15" s="10">
+        <v>400</v>
+      </c>
+      <c r="E15" s="10">
+        <v>400</v>
+      </c>
+      <c r="F15" s="8" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
+      <c r="G15" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="H15" s="10">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="24.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="F16" s="2" t="s">
+      <c r="B16" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D16" s="10">
+        <v>400</v>
+      </c>
+      <c r="E16" s="10">
+        <v>400</v>
+      </c>
+      <c r="F16" s="8" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
+      <c r="G16" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="H16" s="10">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="8" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
+      <c r="B17" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D17" s="10">
+        <v>400</v>
+      </c>
+      <c r="E17" s="10">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="19" x14ac:dyDescent="0.2">
+      <c r="A18" s="8" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" s="5" t="s">
+      <c r="B18" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" s="10">
+        <v>400</v>
+      </c>
+      <c r="E18" s="10">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="13" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" s="5" t="s">
+      <c r="B19" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" s="10">
+        <v>400</v>
+      </c>
+      <c r="E19" s="10">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="13" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21" s="5" t="s">
+      <c r="B20" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" s="10">
+        <v>400</v>
+      </c>
+      <c r="E20" s="10">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="13" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A22" s="5" t="s">
+      <c r="B21" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" s="10">
+        <v>400</v>
+      </c>
+      <c r="E21" s="10">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="13" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A23" s="5" t="s">
+      <c r="B22" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D22" s="10">
+        <v>400</v>
+      </c>
+      <c r="E22" s="10">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="13" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A24" s="5" t="s">
+      <c r="B23" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D23" s="10">
+        <v>400</v>
+      </c>
+      <c r="E23" s="10">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="13" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A25" s="5" t="s">
+      <c r="B24" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="D24" s="10">
+        <v>400</v>
+      </c>
+      <c r="E24" s="10">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="13" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A26" s="5" t="s">
+      <c r="B25" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="D25" s="10">
+        <v>400</v>
+      </c>
+      <c r="E25" s="10">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="13" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A27" s="5" t="s">
+      <c r="B26" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="D26" s="10">
+        <v>400</v>
+      </c>
+      <c r="E26" s="10">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="13" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A28" s="2" t="s">
+      <c r="B27" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="D27" s="10">
+        <v>400</v>
+      </c>
+      <c r="E27" s="10">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="19" x14ac:dyDescent="0.2">
+      <c r="A28" s="8" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A29" s="2" t="s">
+      <c r="B28" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="D28" s="10">
+        <v>400</v>
+      </c>
+      <c r="E28" s="10">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="8" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A30" s="2" t="s">
+      <c r="B29" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="D29" s="10">
+        <v>400</v>
+      </c>
+      <c r="E29" s="10">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="19" x14ac:dyDescent="0.2">
+      <c r="A30" s="8" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A31" s="2" t="s">
+      <c r="B30" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D30" s="10">
+        <v>500</v>
+      </c>
+      <c r="E30" s="10">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="19" x14ac:dyDescent="0.2">
+      <c r="A31" s="8" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A32" s="2" t="s">
+      <c r="B31" s="8" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A33" s="2" t="s">
+      <c r="D31" s="10">
+        <v>600</v>
+      </c>
+      <c r="E31" s="10">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="19" x14ac:dyDescent="0.2">
+      <c r="A32" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D32" s="10">
+        <v>600</v>
+      </c>
+      <c r="E32" s="10">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="19" x14ac:dyDescent="0.2">
+      <c r="A33" s="8" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A34" s="2" t="s">
+      <c r="B33" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D33" s="10">
+        <v>500</v>
+      </c>
+      <c r="E33" s="10">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="19" x14ac:dyDescent="0.2">
+      <c r="A34" s="8" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A35" s="2" t="s">
+      <c r="B34" s="8" t="s">
         <v>45</v>
+      </c>
+      <c r="D34" s="10">
+        <v>600</v>
+      </c>
+      <c r="E34" s="10">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="19" x14ac:dyDescent="0.2">
+      <c r="A35" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D35" s="10">
+        <v>600</v>
+      </c>
+      <c r="E35" s="10">
+        <v>600</v>
       </c>
     </row>
   </sheetData>
@@ -851,36 +1279,43 @@
   <dimension ref="A1:AMJ35"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.33203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="17.6640625" style="1" customWidth="1"/>
-    <col min="3" max="4" width="11.5" style="1"/>
+    <col min="1" max="1" width="29.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.1640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5" style="1"/>
     <col min="5" max="5" width="8.5" style="1" customWidth="1"/>
     <col min="6" max="6" width="20.33203125" style="1" customWidth="1"/>
     <col min="7" max="1024" width="11.5" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="2"/>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="11"/>
-    </row>
-    <row r="2" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C1" s="7"/>
+      <c r="D1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4"/>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="6" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="19" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -890,8 +1325,11 @@
       <c r="F3" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G3" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="19" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
@@ -901,8 +1339,11 @@
       <c r="F4" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G4" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="19" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -912,8 +1353,11 @@
       <c r="F5" s="2" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G5" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="19" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
@@ -923,180 +1367,330 @@
       <c r="F6" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G6" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="19" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="B7" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="F7" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G7" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="19" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="B8" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="F8" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G8" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="19" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="B9" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="F9" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G9" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="19" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="B10" s="1" t="s">
+        <v>47</v>
+      </c>
       <c r="F10" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G10" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="19" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>18</v>
       </c>
+      <c r="B11" s="1" t="s">
+        <v>47</v>
+      </c>
       <c r="F11" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G11" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="B12" s="1" t="s">
+        <v>48</v>
+      </c>
       <c r="F12" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G12" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="19" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="B13" s="1" t="s">
+        <v>48</v>
+      </c>
       <c r="F13" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G13" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="19" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="B14" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="F14" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G14" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="19" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="B15" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="F15" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G15" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="24.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="B16" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="F16" s="2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G16" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" ht="17" x14ac:dyDescent="0.2">
+      <c r="B17" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B18" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B19" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B21" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B22" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B23" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B24" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B25" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B26" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" ht="17" x14ac:dyDescent="0.2">
+      <c r="B27" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" ht="17" x14ac:dyDescent="0.2">
+      <c r="B28" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" ht="17" x14ac:dyDescent="0.2">
+      <c r="B29" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" ht="17" x14ac:dyDescent="0.2">
+      <c r="B30" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" ht="17" x14ac:dyDescent="0.2">
+      <c r="B31" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" ht="17" x14ac:dyDescent="0.2">
+      <c r="B32" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="19" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" ht="17" x14ac:dyDescent="0.2">
+      <c r="B33" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="19" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" ht="17" x14ac:dyDescent="0.2">
+      <c r="B34" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="19" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>45</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -1117,412 +1711,660 @@
   <dimension ref="A1:AMJ35"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="29.5" style="6" customWidth="1"/>
-    <col min="2" max="2" width="20.6640625" style="6" customWidth="1"/>
-    <col min="3" max="3" width="15.1640625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="11.5" style="6"/>
-    <col min="5" max="5" width="8.5" style="6" customWidth="1"/>
-    <col min="6" max="6" width="20.33203125" style="6" customWidth="1"/>
-    <col min="7" max="1024" width="11.5" style="6"/>
+    <col min="1" max="1" width="29.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.1640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5" style="1"/>
+    <col min="5" max="5" width="8.5" style="1" customWidth="1"/>
+    <col min="6" max="6" width="20.33203125" style="1" customWidth="1"/>
+    <col min="7" max="1024" width="11.5" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="7"/>
-      <c r="B1" s="12" t="s">
+    <row r="1" spans="1:8" ht="19" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="12"/>
-    </row>
-    <row r="2" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="9"/>
-      <c r="B2" s="8" t="s">
+      <c r="C1" s="7"/>
+      <c r="D1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="4"/>
+      <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="19" x14ac:dyDescent="0.2">
-      <c r="A3" s="7" t="s">
+    <row r="3" spans="1:8" ht="19" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="D3" s="1">
+        <v>300</v>
+      </c>
+      <c r="E3" s="1">
+        <v>300</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="6" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="19" x14ac:dyDescent="0.2">
-      <c r="A4" s="7" t="s">
+      <c r="G3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H3" s="1">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="19" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="D4" s="1">
+        <v>300</v>
+      </c>
+      <c r="E4" s="1">
+        <v>300</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="6" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="19" x14ac:dyDescent="0.2">
-      <c r="A5" s="7" t="s">
+      <c r="G4" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H4" s="1">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="19" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="D5" s="1">
+        <v>300</v>
+      </c>
+      <c r="E5" s="1">
+        <v>300</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G5" s="6" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="19" x14ac:dyDescent="0.2">
-      <c r="A6" s="7" t="s">
+      <c r="G5" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H5" s="1">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="19" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="D6" s="1">
+        <v>300</v>
+      </c>
+      <c r="E6" s="1">
+        <v>300</v>
+      </c>
+      <c r="F6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="6" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="19" x14ac:dyDescent="0.2">
-      <c r="A7" s="7" t="s">
+      <c r="G6" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H6" s="1">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="19" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="D7" s="1">
+        <v>300</v>
+      </c>
+      <c r="E7" s="1">
+        <v>300</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G7" s="6" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="19" x14ac:dyDescent="0.2">
-      <c r="A8" s="7" t="s">
+      <c r="G7" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H7" s="1">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="19" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F8" s="7" t="s">
+      <c r="D8" s="1">
+        <v>300</v>
+      </c>
+      <c r="E8" s="1">
+        <v>300</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="6" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="19" x14ac:dyDescent="0.2">
-      <c r="A9" s="7" t="s">
+      <c r="G8" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H8" s="1">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="19" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F9" s="7" t="s">
+      <c r="D9" s="1">
+        <v>300</v>
+      </c>
+      <c r="E9" s="1">
+        <v>300</v>
+      </c>
+      <c r="F9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G9" s="6" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="19" x14ac:dyDescent="0.2">
-      <c r="A10" s="7" t="s">
+      <c r="G9" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H9" s="1">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="19" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="F10" s="7" t="s">
+      <c r="D10" s="1">
+        <v>300</v>
+      </c>
+      <c r="E10" s="1">
+        <v>300</v>
+      </c>
+      <c r="F10" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G10" s="6" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="19" x14ac:dyDescent="0.2">
-      <c r="A11" s="7" t="s">
+      <c r="G10" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H10" s="1">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="19" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="F11" s="7" t="s">
+      <c r="D11" s="1">
+        <v>300</v>
+      </c>
+      <c r="E11" s="1">
+        <v>300</v>
+      </c>
+      <c r="F11" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G11" s="6" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="7" t="s">
+      <c r="G11" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H11" s="1">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="F12" s="7" t="s">
+      <c r="D12" s="1">
+        <v>400</v>
+      </c>
+      <c r="E12" s="1">
+        <v>400</v>
+      </c>
+      <c r="F12" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="G12" s="6" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="19" x14ac:dyDescent="0.2">
-      <c r="A13" s="7" t="s">
+      <c r="G12" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H12" s="1">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="19" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="F13" s="7" t="s">
+      <c r="D13" s="1">
+        <v>400</v>
+      </c>
+      <c r="E13" s="1">
+        <v>400</v>
+      </c>
+      <c r="F13" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="G13" s="6" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="19" x14ac:dyDescent="0.2">
-      <c r="A14" s="7" t="s">
+      <c r="G13" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H13" s="1">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="19" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F14" s="7" t="s">
+      <c r="D14" s="1">
+        <v>400</v>
+      </c>
+      <c r="E14" s="1">
+        <v>400</v>
+      </c>
+      <c r="F14" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="G14" s="6" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="19" x14ac:dyDescent="0.2">
-      <c r="A15" s="7" t="s">
+      <c r="G14" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H14" s="1">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="19" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F15" s="7" t="s">
+      <c r="D15" s="1">
+        <v>400</v>
+      </c>
+      <c r="E15" s="1">
+        <v>400</v>
+      </c>
+      <c r="F15" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="G15" s="6" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="24.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="7" t="s">
+      <c r="G15" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H15" s="1">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="24.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F16" s="7" t="s">
+      <c r="D16" s="1">
+        <v>400</v>
+      </c>
+      <c r="E16" s="1">
+        <v>400</v>
+      </c>
+      <c r="F16" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G16" s="6" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="7" t="s">
+      <c r="G16" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H16" s="1">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" ht="19" x14ac:dyDescent="0.2">
-      <c r="A18" s="7" t="s">
+      <c r="D17" s="1">
+        <v>400</v>
+      </c>
+      <c r="E17" s="1">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="19" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="10" t="s">
+      <c r="D18" s="1">
+        <v>300</v>
+      </c>
+      <c r="E18" s="1">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="10" t="s">
+      <c r="D19" s="1">
+        <v>300</v>
+      </c>
+      <c r="E19" s="1">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="C20" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="10" t="s">
+      <c r="D20" s="1">
+        <v>300</v>
+      </c>
+      <c r="E20" s="1">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="B21" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="C21" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" s="10" t="s">
+      <c r="D21" s="1">
+        <v>300</v>
+      </c>
+      <c r="E21" s="1">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="B22" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C22" s="6" t="s">
+      <c r="C22" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="10" t="s">
+      <c r="D22" s="1">
+        <v>300</v>
+      </c>
+      <c r="E22" s="1">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="B23" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C23" s="6" t="s">
+      <c r="C23" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" s="10" t="s">
+      <c r="D23" s="1">
+        <v>300</v>
+      </c>
+      <c r="E23" s="1">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B24" s="6" t="s">
+      <c r="B24" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C24" s="6" t="s">
+      <c r="C24" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="10" t="s">
+      <c r="D24" s="1">
+        <v>300</v>
+      </c>
+      <c r="E24" s="1">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="B25" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C25" s="6" t="s">
+      <c r="C25" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" s="10" t="s">
+      <c r="D25" s="1">
+        <v>300</v>
+      </c>
+      <c r="E25" s="1">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B26" s="6" t="s">
+      <c r="B26" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C26" s="6" t="s">
+      <c r="C26" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" s="10" t="s">
+      <c r="D26" s="1">
+        <v>300</v>
+      </c>
+      <c r="E26" s="1">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="B27" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C27" s="6" t="s">
+      <c r="C27" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" ht="19" x14ac:dyDescent="0.2">
-      <c r="A28" s="7" t="s">
+      <c r="D27" s="1">
+        <v>400</v>
+      </c>
+      <c r="E27" s="1">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="19" x14ac:dyDescent="0.2">
+      <c r="A28" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B28" s="6" t="s">
+      <c r="B28" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="7" t="s">
+      <c r="D28" s="1">
+        <v>400</v>
+      </c>
+      <c r="E28" s="1">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B29" s="6" t="s">
+      <c r="B29" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" ht="19" x14ac:dyDescent="0.2">
-      <c r="A30" s="7" t="s">
+      <c r="D29" s="1">
+        <v>400</v>
+      </c>
+      <c r="E29" s="1">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="19" x14ac:dyDescent="0.2">
+      <c r="A30" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B30" s="6" t="s">
+      <c r="B30" s="1" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" ht="19" x14ac:dyDescent="0.2">
-      <c r="A31" s="7" t="s">
+      <c r="D30" s="1">
+        <v>500</v>
+      </c>
+      <c r="E30" s="1">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="19" x14ac:dyDescent="0.2">
+      <c r="A31" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B31" s="6" t="s">
+      <c r="B31" s="1" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" ht="19" x14ac:dyDescent="0.2">
-      <c r="A32" s="7" t="s">
+      <c r="D31" s="1">
+        <v>500</v>
+      </c>
+      <c r="E31" s="1">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="19" x14ac:dyDescent="0.2">
+      <c r="A32" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B32" s="6" t="s">
+      <c r="B32" s="1" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" ht="19" x14ac:dyDescent="0.2">
-      <c r="A33" s="7" t="s">
+      <c r="D32" s="1">
+        <v>500</v>
+      </c>
+      <c r="E32" s="1">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="19" x14ac:dyDescent="0.2">
+      <c r="A33" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B33" s="6" t="s">
+      <c r="B33" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" ht="19" x14ac:dyDescent="0.2">
-      <c r="A34" s="7" t="s">
+      <c r="D33" s="1">
+        <v>400</v>
+      </c>
+      <c r="E33" s="1">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="19" x14ac:dyDescent="0.2">
+      <c r="A34" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B34" s="6" t="s">
+      <c r="B34" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" ht="19" x14ac:dyDescent="0.2">
-      <c r="A35" s="7" t="s">
+      <c r="D34" s="1">
+        <v>400</v>
+      </c>
+      <c r="E34" s="1">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="19" x14ac:dyDescent="0.2">
+      <c r="A35" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B35" s="6" t="s">
+      <c r="B35" s="1" t="s">
         <v>49</v>
+      </c>
+      <c r="D35" s="1">
+        <v>400</v>
+      </c>
+      <c r="E35" s="1">
+        <v>400</v>
       </c>
     </row>
   </sheetData>
@@ -1543,252 +2385,660 @@
   <dimension ref="A1:AMJ35"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.33203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="17.6640625" style="1" customWidth="1"/>
-    <col min="3" max="4" width="11.5" style="1"/>
+    <col min="1" max="1" width="29.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.1640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5" style="1"/>
     <col min="5" max="5" width="8.5" style="1" customWidth="1"/>
     <col min="6" max="6" width="20.33203125" style="1" customWidth="1"/>
     <col min="7" max="1024" width="11.5" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="2"/>
-      <c r="B1" s="11" t="s">
+    <row r="1" spans="1:8" ht="19" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="11"/>
-    </row>
-    <row r="2" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C1" s="7"/>
+      <c r="D1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4"/>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="6" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="19" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="D3" s="1">
+        <v>250</v>
+      </c>
+      <c r="E3" s="1">
+        <v>250</v>
+      </c>
       <c r="F3" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H3" s="1">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="19" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="D4" s="1">
+        <v>250</v>
+      </c>
+      <c r="E4" s="1">
+        <v>250</v>
+      </c>
       <c r="F4" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G4" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H4" s="1">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="19" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="D5" s="1">
+        <v>250</v>
+      </c>
+      <c r="E5" s="1">
+        <v>250</v>
+      </c>
       <c r="F5" s="2" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G5" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H5" s="1">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="19" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="D6" s="1">
+        <v>250</v>
+      </c>
+      <c r="E6" s="1">
+        <v>250</v>
+      </c>
       <c r="F6" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G6" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H6" s="1">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="19" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="B7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="1">
+        <v>250</v>
+      </c>
+      <c r="E7" s="1">
+        <v>250</v>
+      </c>
       <c r="F7" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G7" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H7" s="1">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="19" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="B8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="1">
+        <v>250</v>
+      </c>
+      <c r="E8" s="1">
+        <v>250</v>
+      </c>
       <c r="F8" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G8" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H8" s="1">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="19" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="B9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="1">
+        <v>250</v>
+      </c>
+      <c r="E9" s="1">
+        <v>250</v>
+      </c>
       <c r="F9" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G9" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H9" s="1">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="19" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="B10" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D10" s="1">
+        <v>250</v>
+      </c>
+      <c r="E10" s="1">
+        <v>250</v>
+      </c>
       <c r="F10" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G10" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H10" s="1">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="19" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>18</v>
       </c>
+      <c r="B11" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D11" s="1">
+        <v>250</v>
+      </c>
+      <c r="E11" s="1">
+        <v>250</v>
+      </c>
       <c r="F11" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G11" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H11" s="1">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="B12" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D12" s="1">
+        <v>350</v>
+      </c>
+      <c r="E12" s="1">
+        <v>350</v>
+      </c>
       <c r="F12" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G12" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H12" s="1">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="19" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="B13" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D13" s="1">
+        <v>350</v>
+      </c>
+      <c r="E13" s="1">
+        <v>350</v>
+      </c>
       <c r="F13" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G13" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H13" s="1">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="19" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="B14" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D14" s="1">
+        <v>350</v>
+      </c>
+      <c r="E14" s="1">
+        <v>350</v>
+      </c>
       <c r="F14" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G14" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H14" s="1">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="19" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="B15" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D15" s="1">
+        <v>350</v>
+      </c>
+      <c r="E15" s="1">
+        <v>350</v>
+      </c>
       <c r="F15" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G15" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H15" s="1">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="24.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="B16" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D16" s="1">
+        <v>350</v>
+      </c>
+      <c r="E16" s="1">
+        <v>350</v>
+      </c>
       <c r="F16" s="2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G16" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H16" s="1">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" ht="17" x14ac:dyDescent="0.2">
+      <c r="B17" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D17" s="1">
+        <v>350</v>
+      </c>
+      <c r="E17" s="1">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B18" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" s="1">
+        <v>250</v>
+      </c>
+      <c r="E18" s="1">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B19" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" s="1">
+        <v>250</v>
+      </c>
+      <c r="E19" s="1">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" s="1">
+        <v>250</v>
+      </c>
+      <c r="E20" s="1">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B21" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" s="1">
+        <v>250</v>
+      </c>
+      <c r="E21" s="1">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B22" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D22" s="1">
+        <v>250</v>
+      </c>
+      <c r="E22" s="1">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B23" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D23" s="1">
+        <v>250</v>
+      </c>
+      <c r="E23" s="1">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B24" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D24" s="1">
+        <v>250</v>
+      </c>
+      <c r="E24" s="1">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B25" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D25" s="1">
+        <v>250</v>
+      </c>
+      <c r="E25" s="1">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B26" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D26" s="1">
+        <v>250</v>
+      </c>
+      <c r="E26" s="1">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" ht="17" x14ac:dyDescent="0.2">
+      <c r="B27" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D27" s="1">
+        <v>350</v>
+      </c>
+      <c r="E27" s="1">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" ht="17" x14ac:dyDescent="0.2">
+      <c r="B28" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D28" s="1">
+        <v>350</v>
+      </c>
+      <c r="E28" s="1">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" ht="17" x14ac:dyDescent="0.2">
+      <c r="B29" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D29" s="1">
+        <v>350</v>
+      </c>
+      <c r="E29" s="1">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" ht="17" x14ac:dyDescent="0.2">
+      <c r="B30" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D30" s="1">
+        <v>500</v>
+      </c>
+      <c r="E30" s="1">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" ht="17" x14ac:dyDescent="0.2">
+      <c r="B31" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D31" s="1">
+        <v>500</v>
+      </c>
+      <c r="E31" s="1">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" ht="17" x14ac:dyDescent="0.2">
+      <c r="B32" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D32" s="1">
+        <v>500</v>
+      </c>
+      <c r="E32" s="1">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" ht="17" x14ac:dyDescent="0.2">
+      <c r="B33" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D33" s="1">
+        <v>350</v>
+      </c>
+      <c r="E33" s="1">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" ht="17" x14ac:dyDescent="0.2">
+      <c r="B34" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D34" s="1">
+        <v>350</v>
+      </c>
+      <c r="E34" s="1">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>45</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D35" s="1">
+        <v>350</v>
+      </c>
+      <c r="E35" s="1">
+        <v>350</v>
       </c>
     </row>
   </sheetData>
@@ -1808,253 +3058,661 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AMJ35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.33203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="17.6640625" style="1" customWidth="1"/>
-    <col min="3" max="4" width="11.5" style="1"/>
+    <col min="1" max="1" width="29.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.1640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5" style="1"/>
     <col min="5" max="5" width="8.5" style="1" customWidth="1"/>
     <col min="6" max="6" width="20.33203125" style="1" customWidth="1"/>
     <col min="7" max="1024" width="11.5" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="2"/>
-      <c r="B1" s="11" t="s">
+    <row r="1" spans="1:8" ht="19" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="11"/>
-    </row>
-    <row r="2" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C1" s="7"/>
+      <c r="D1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4"/>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="6" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="19" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="D3" s="1">
+        <v>250</v>
+      </c>
+      <c r="E3" s="1">
+        <v>250</v>
+      </c>
       <c r="F3" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H3" s="1">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="19" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="D4" s="1">
+        <v>250</v>
+      </c>
+      <c r="E4" s="1">
+        <v>250</v>
+      </c>
       <c r="F4" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G4" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H4" s="1">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="19" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="D5" s="1">
+        <v>250</v>
+      </c>
+      <c r="E5" s="1">
+        <v>250</v>
+      </c>
       <c r="F5" s="2" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G5" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H5" s="1">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="19" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="D6" s="1">
+        <v>250</v>
+      </c>
+      <c r="E6" s="1">
+        <v>250</v>
+      </c>
       <c r="F6" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G6" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H6" s="1">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="19" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="B7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="1">
+        <v>250</v>
+      </c>
+      <c r="E7" s="1">
+        <v>250</v>
+      </c>
       <c r="F7" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G7" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H7" s="1">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="19" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="B8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="1">
+        <v>250</v>
+      </c>
+      <c r="E8" s="1">
+        <v>250</v>
+      </c>
       <c r="F8" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G8" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H8" s="1">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="19" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="B9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="1">
+        <v>250</v>
+      </c>
+      <c r="E9" s="1">
+        <v>250</v>
+      </c>
       <c r="F9" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G9" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H9" s="1">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="19" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="B10" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D10" s="1">
+        <v>250</v>
+      </c>
+      <c r="E10" s="1">
+        <v>250</v>
+      </c>
       <c r="F10" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G10" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H10" s="1">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="19" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>18</v>
       </c>
+      <c r="B11" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D11" s="1">
+        <v>250</v>
+      </c>
+      <c r="E11" s="1">
+        <v>250</v>
+      </c>
       <c r="F11" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G11" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H11" s="1">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="22.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="B12" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D12" s="1">
+        <v>350</v>
+      </c>
+      <c r="E12" s="1">
+        <v>350</v>
+      </c>
       <c r="F12" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G12" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H12" s="1">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="19" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="B13" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D13" s="1">
+        <v>350</v>
+      </c>
+      <c r="E13" s="1">
+        <v>350</v>
+      </c>
       <c r="F13" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G13" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H13" s="1">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="19" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="B14" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D14" s="1">
+        <v>350</v>
+      </c>
+      <c r="E14" s="1">
+        <v>350</v>
+      </c>
       <c r="F14" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G14" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H14" s="1">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="19" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="B15" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D15" s="1">
+        <v>350</v>
+      </c>
+      <c r="E15" s="1">
+        <v>350</v>
+      </c>
       <c r="F15" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G15" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H15" s="1">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="24.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="B16" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D16" s="1">
+        <v>350</v>
+      </c>
+      <c r="E16" s="1">
+        <v>350</v>
+      </c>
       <c r="F16" s="2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G16" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H16" s="1">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" ht="17" x14ac:dyDescent="0.2">
+      <c r="B17" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D17" s="1">
+        <v>350</v>
+      </c>
+      <c r="E17" s="1">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B18" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" s="1">
+        <v>250</v>
+      </c>
+      <c r="E18" s="1">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B19" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" s="1">
+        <v>250</v>
+      </c>
+      <c r="E19" s="1">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" s="1">
+        <v>250</v>
+      </c>
+      <c r="E20" s="1">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B21" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" s="1">
+        <v>250</v>
+      </c>
+      <c r="E21" s="1">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B22" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D22" s="1">
+        <v>250</v>
+      </c>
+      <c r="E22" s="1">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B23" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D23" s="1">
+        <v>250</v>
+      </c>
+      <c r="E23" s="1">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B24" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D24" s="1">
+        <v>250</v>
+      </c>
+      <c r="E24" s="1">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B25" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D25" s="1">
+        <v>250</v>
+      </c>
+      <c r="E25" s="1">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B26" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D26" s="1">
+        <v>250</v>
+      </c>
+      <c r="E26" s="1">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" ht="17" x14ac:dyDescent="0.2">
+      <c r="B27" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D27" s="1">
+        <v>350</v>
+      </c>
+      <c r="E27" s="1">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" ht="17" x14ac:dyDescent="0.2">
+      <c r="B28" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D28" s="1">
+        <v>350</v>
+      </c>
+      <c r="E28" s="1">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" ht="17" x14ac:dyDescent="0.2">
+      <c r="B29" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D29" s="1">
+        <v>350</v>
+      </c>
+      <c r="E29" s="1">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" ht="17" x14ac:dyDescent="0.2">
+      <c r="B30" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D30" s="1">
+        <v>500</v>
+      </c>
+      <c r="E30" s="1">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" ht="17" x14ac:dyDescent="0.2">
+      <c r="B31" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D31" s="1">
+        <v>500</v>
+      </c>
+      <c r="E31" s="1">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" ht="17" x14ac:dyDescent="0.2">
+      <c r="B32" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D32" s="1">
+        <v>500</v>
+      </c>
+      <c r="E32" s="1">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" ht="17" x14ac:dyDescent="0.2">
+      <c r="B33" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D33" s="1">
+        <v>350</v>
+      </c>
+      <c r="E33" s="1">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" ht="17" x14ac:dyDescent="0.2">
+      <c r="B34" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D34" s="1">
+        <v>350</v>
+      </c>
+      <c r="E34" s="1">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>45</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D35" s="1">
+        <v>350</v>
+      </c>
+      <c r="E35" s="1">
+        <v>350</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
nově zpracované kategorie v závodě a startovné
</commit_message>
<xml_diff>
--- a/static/classes/classes.xlsx
+++ b/static/classes/classes.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="664" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="664" uniqueCount="59">
   <si>
     <t xml:space="preserve">MČR</t>
   </si>
@@ -183,6 +183,12 @@
   </si>
   <si>
     <t xml:space="preserve">Women Elite</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cruiser TOP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cruiser 40+</t>
   </si>
   <si>
     <t xml:space="preserve">Men Junior/Elite</t>
@@ -204,7 +210,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -250,6 +256,11 @@
       <family val="1"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -293,7 +304,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -342,6 +353,10 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -366,16 +381,16 @@
   <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C28" activeCellId="1" sqref="C3:C17 C28"/>
+      <selection pane="topLeft" activeCell="C28" activeCellId="1" sqref="G3:G16 C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.515625" defaultRowHeight="18" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="29.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="20.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="20.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15.15"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="11.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="8.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="8.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="20.33"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="7" style="1" width="11.5"/>
   </cols>
@@ -1097,10 +1112,10 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Běžné"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Běžné"&amp;12Stránka &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Stránka &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -1112,19 +1127,20 @@
   </sheetPr>
   <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3:C17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3:G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.515625" defaultRowHeight="18" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="7" width="29.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="7" width="20.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="7" width="15.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="7" width="20.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="7" width="15.15"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="7" width="11.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="7" width="8.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="7" width="8.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="7" width="20.33"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="7" style="7" width="11.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="7" width="20.83"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="8" style="7" width="11.5"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1163,7 +1179,7 @@
         <v>6</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>7</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1179,8 +1195,8 @@
       <c r="F4" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="7" t="s">
-        <v>7</v>
+      <c r="G4" s="12" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1196,8 +1212,8 @@
       <c r="F5" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="7" t="s">
-        <v>7</v>
+      <c r="G5" s="12" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1213,8 +1229,8 @@
       <c r="F6" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="7" t="s">
-        <v>7</v>
+      <c r="G6" s="12" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1230,8 +1246,8 @@
       <c r="F7" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="G7" s="7" t="s">
-        <v>7</v>
+      <c r="G7" s="12" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1247,8 +1263,8 @@
       <c r="F8" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="G8" s="7" t="s">
-        <v>7</v>
+      <c r="G8" s="12" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1264,8 +1280,8 @@
       <c r="F9" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="G9" s="7" t="s">
-        <v>7</v>
+      <c r="G9" s="12" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1282,7 +1298,7 @@
         <v>22</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>7</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1298,8 +1314,8 @@
       <c r="F11" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="G11" s="7" t="s">
-        <v>7</v>
+      <c r="G11" s="12" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="22.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1315,8 +1331,8 @@
       <c r="F12" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="G12" s="7" t="s">
-        <v>7</v>
+      <c r="G12" s="12" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1332,8 +1348,8 @@
       <c r="F13" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="G13" s="7" t="s">
-        <v>7</v>
+      <c r="G13" s="12" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1349,11 +1365,11 @@
       <c r="F14" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="G14" s="7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G14" s="12" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="27.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="8" t="s">
         <v>15</v>
       </c>
@@ -1366,11 +1382,11 @@
       <c r="F15" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="G15" s="7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="24.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G15" s="12" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="36.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="8" t="s">
         <v>17</v>
       </c>
@@ -1383,8 +1399,8 @@
       <c r="F16" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="G16" s="7" t="s">
-        <v>7</v>
+      <c r="G16" s="12" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1410,7 +1426,7 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="12" t="s">
+      <c r="A19" s="13" t="s">
         <v>36</v>
       </c>
       <c r="B19" s="7" t="s">
@@ -1421,7 +1437,7 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="12" t="s">
+      <c r="A20" s="13" t="s">
         <v>37</v>
       </c>
       <c r="B20" s="7" t="s">
@@ -1432,7 +1448,7 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="12" t="s">
+      <c r="A21" s="13" t="s">
         <v>38</v>
       </c>
       <c r="B21" s="7" t="s">
@@ -1443,7 +1459,7 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="12" t="s">
+      <c r="A22" s="13" t="s">
         <v>39</v>
       </c>
       <c r="B22" s="7" t="s">
@@ -1454,7 +1470,7 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="12" t="s">
+      <c r="A23" s="13" t="s">
         <v>40</v>
       </c>
       <c r="B23" s="7" t="s">
@@ -1465,7 +1481,7 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="12" t="s">
+      <c r="A24" s="13" t="s">
         <v>41</v>
       </c>
       <c r="B24" s="7" t="s">
@@ -1476,7 +1492,7 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="12" t="s">
+      <c r="A25" s="13" t="s">
         <v>42</v>
       </c>
       <c r="B25" s="7" t="s">
@@ -1487,7 +1503,7 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="12" t="s">
+      <c r="A26" s="13" t="s">
         <v>43</v>
       </c>
       <c r="B26" s="7" t="s">
@@ -1498,7 +1514,7 @@
       </c>
     </row>
     <row r="27" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="12" t="s">
+      <c r="A27" s="13" t="s">
         <v>44</v>
       </c>
       <c r="B27" s="7" t="s">
@@ -1535,10 +1551,10 @@
         <v>47</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1546,10 +1562,10 @@
         <v>48</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1557,10 +1573,10 @@
         <v>49</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1602,10 +1618,10 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Běžné"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Běžné"&amp;12Stránka &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Stránka &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -1617,24 +1633,25 @@
   </sheetPr>
   <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C28" activeCellId="1" sqref="C3:C17 C28"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3:G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.515625" defaultRowHeight="18" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="7" width="29.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="7" width="20.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="7" width="15.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="7" width="20.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="7" width="15.15"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="7" width="11.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="7" width="8.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="7" width="8.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="7" width="20.33"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="7" style="7" width="11.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="7" width="22.79"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="8" style="7" width="11.5"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="8" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>1</v>
@@ -1676,7 +1693,7 @@
         <v>6</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>7</v>
+        <v>53</v>
       </c>
       <c r="H3" s="7" t="n">
         <v>300</v>
@@ -1701,8 +1718,8 @@
       <c r="F4" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="7" t="s">
-        <v>7</v>
+      <c r="G4" s="12" t="s">
+        <v>53</v>
       </c>
       <c r="H4" s="7" t="n">
         <v>300</v>
@@ -1727,8 +1744,8 @@
       <c r="F5" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="7" t="s">
-        <v>7</v>
+      <c r="G5" s="12" t="s">
+        <v>53</v>
       </c>
       <c r="H5" s="7" t="n">
         <v>300</v>
@@ -1753,8 +1770,8 @@
       <c r="F6" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="7" t="s">
-        <v>7</v>
+      <c r="G6" s="12" t="s">
+        <v>53</v>
       </c>
       <c r="H6" s="7" t="n">
         <v>300</v>
@@ -1779,8 +1796,8 @@
       <c r="F7" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="G7" s="7" t="s">
-        <v>7</v>
+      <c r="G7" s="12" t="s">
+        <v>53</v>
       </c>
       <c r="H7" s="7" t="n">
         <v>300</v>
@@ -1805,8 +1822,8 @@
       <c r="F8" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="G8" s="7" t="s">
-        <v>7</v>
+      <c r="G8" s="12" t="s">
+        <v>53</v>
       </c>
       <c r="H8" s="7" t="n">
         <v>300</v>
@@ -1831,8 +1848,8 @@
       <c r="F9" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="G9" s="7" t="s">
-        <v>7</v>
+      <c r="G9" s="12" t="s">
+        <v>53</v>
       </c>
       <c r="H9" s="7" t="n">
         <v>300</v>
@@ -1858,7 +1875,7 @@
         <v>22</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>7</v>
+        <v>54</v>
       </c>
       <c r="H10" s="7" t="n">
         <v>300</v>
@@ -1883,8 +1900,8 @@
       <c r="F11" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="G11" s="7" t="s">
-        <v>7</v>
+      <c r="G11" s="12" t="s">
+        <v>54</v>
       </c>
       <c r="H11" s="7" t="n">
         <v>300</v>
@@ -1909,8 +1926,8 @@
       <c r="F12" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="G12" s="7" t="s">
-        <v>7</v>
+      <c r="G12" s="12" t="s">
+        <v>53</v>
       </c>
       <c r="H12" s="7" t="n">
         <v>300</v>
@@ -1935,8 +1952,8 @@
       <c r="F13" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="G13" s="7" t="s">
-        <v>7</v>
+      <c r="G13" s="12" t="s">
+        <v>53</v>
       </c>
       <c r="H13" s="7" t="n">
         <v>300</v>
@@ -1961,8 +1978,8 @@
       <c r="F14" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="G14" s="7" t="s">
-        <v>7</v>
+      <c r="G14" s="12" t="s">
+        <v>53</v>
       </c>
       <c r="H14" s="7" t="n">
         <v>300</v>
@@ -1987,8 +2004,8 @@
       <c r="F15" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="G15" s="7" t="s">
-        <v>7</v>
+      <c r="G15" s="12" t="s">
+        <v>53</v>
       </c>
       <c r="H15" s="7" t="n">
         <v>300</v>
@@ -2013,8 +2030,8 @@
       <c r="F16" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="G16" s="7" t="s">
-        <v>7</v>
+      <c r="G16" s="12" t="s">
+        <v>54</v>
       </c>
       <c r="H16" s="7" t="n">
         <v>300</v>
@@ -2055,7 +2072,7 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="12" t="s">
+      <c r="A19" s="13" t="s">
         <v>36</v>
       </c>
       <c r="B19" s="7" t="s">
@@ -2072,7 +2089,7 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="12" t="s">
+      <c r="A20" s="13" t="s">
         <v>37</v>
       </c>
       <c r="B20" s="7" t="s">
@@ -2089,7 +2106,7 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="12" t="s">
+      <c r="A21" s="13" t="s">
         <v>38</v>
       </c>
       <c r="B21" s="7" t="s">
@@ -2106,7 +2123,7 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="12" t="s">
+      <c r="A22" s="13" t="s">
         <v>39</v>
       </c>
       <c r="B22" s="7" t="s">
@@ -2123,7 +2140,7 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="12" t="s">
+      <c r="A23" s="13" t="s">
         <v>40</v>
       </c>
       <c r="B23" s="7" t="s">
@@ -2140,7 +2157,7 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="12" t="s">
+      <c r="A24" s="13" t="s">
         <v>41</v>
       </c>
       <c r="B24" s="7" t="s">
@@ -2157,7 +2174,7 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="12" t="s">
+      <c r="A25" s="13" t="s">
         <v>42</v>
       </c>
       <c r="B25" s="7" t="s">
@@ -2174,7 +2191,7 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="12" t="s">
+      <c r="A26" s="13" t="s">
         <v>43</v>
       </c>
       <c r="B26" s="7" t="s">
@@ -2191,7 +2208,7 @@
       </c>
     </row>
     <row r="27" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="12" t="s">
+      <c r="A27" s="13" t="s">
         <v>44</v>
       </c>
       <c r="B27" s="7" t="s">
@@ -2246,10 +2263,10 @@
         <v>47</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D30" s="7" t="n">
         <v>500</v>
@@ -2263,10 +2280,10 @@
         <v>48</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D31" s="7" t="n">
         <v>500</v>
@@ -2280,10 +2297,10 @@
         <v>49</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D32" s="7" t="n">
         <v>500</v>
@@ -2349,10 +2366,10 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Běžné"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Běžné"&amp;12Stránka &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Stránka &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -2365,23 +2382,23 @@
   <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C28" activeCellId="1" sqref="C3:C17 C28"/>
+      <selection pane="topLeft" activeCell="C28" activeCellId="1" sqref="G3:G16 C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.515625" defaultRowHeight="18" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="7" width="29.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="7" width="20.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="7" width="15.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="7" width="20.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="7" width="15.15"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="7" width="11.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="7" width="8.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="7" width="8.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="7" width="20.33"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="7" style="7" width="11.5"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="8" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>1</v>
@@ -2802,7 +2819,7 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="12" t="s">
+      <c r="A19" s="13" t="s">
         <v>36</v>
       </c>
       <c r="B19" s="7" t="s">
@@ -2819,7 +2836,7 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="12" t="s">
+      <c r="A20" s="13" t="s">
         <v>37</v>
       </c>
       <c r="B20" s="7" t="s">
@@ -2836,7 +2853,7 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="12" t="s">
+      <c r="A21" s="13" t="s">
         <v>38</v>
       </c>
       <c r="B21" s="7" t="s">
@@ -2853,7 +2870,7 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="12" t="s">
+      <c r="A22" s="13" t="s">
         <v>39</v>
       </c>
       <c r="B22" s="7" t="s">
@@ -2870,7 +2887,7 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="12" t="s">
+      <c r="A23" s="13" t="s">
         <v>40</v>
       </c>
       <c r="B23" s="7" t="s">
@@ -2887,7 +2904,7 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="12" t="s">
+      <c r="A24" s="13" t="s">
         <v>41</v>
       </c>
       <c r="B24" s="7" t="s">
@@ -2904,7 +2921,7 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="12" t="s">
+      <c r="A25" s="13" t="s">
         <v>42</v>
       </c>
       <c r="B25" s="7" t="s">
@@ -2921,7 +2938,7 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="12" t="s">
+      <c r="A26" s="13" t="s">
         <v>43</v>
       </c>
       <c r="B26" s="7" t="s">
@@ -2938,7 +2955,7 @@
       </c>
     </row>
     <row r="27" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="12" t="s">
+      <c r="A27" s="13" t="s">
         <v>44</v>
       </c>
       <c r="B27" s="7" t="s">
@@ -2993,10 +3010,10 @@
         <v>47</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D30" s="7" t="n">
         <v>500</v>
@@ -3010,10 +3027,10 @@
         <v>48</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D31" s="7" t="n">
         <v>500</v>
@@ -3027,10 +3044,10 @@
         <v>49</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D32" s="7" t="n">
         <v>500</v>
@@ -3096,10 +3113,10 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Běžné"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Běžné"&amp;12Stránka &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Stránka &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -3112,23 +3129,23 @@
   <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3:C17"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="1" sqref="G3:G16 C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.515625" defaultRowHeight="18" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="7" width="29.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="7" width="20.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="7" width="15.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="7" width="20.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="7" width="15.15"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="7" width="11.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="7" width="8.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="7" width="8.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="7" width="20.33"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="7" style="7" width="11.5"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="8" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>1</v>
@@ -3549,7 +3566,7 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="12" t="s">
+      <c r="A19" s="13" t="s">
         <v>36</v>
       </c>
       <c r="B19" s="7" t="s">
@@ -3566,7 +3583,7 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="12" t="s">
+      <c r="A20" s="13" t="s">
         <v>37</v>
       </c>
       <c r="B20" s="7" t="s">
@@ -3583,7 +3600,7 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="12" t="s">
+      <c r="A21" s="13" t="s">
         <v>38</v>
       </c>
       <c r="B21" s="7" t="s">
@@ -3600,7 +3617,7 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="12" t="s">
+      <c r="A22" s="13" t="s">
         <v>39</v>
       </c>
       <c r="B22" s="7" t="s">
@@ -3617,7 +3634,7 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="12" t="s">
+      <c r="A23" s="13" t="s">
         <v>40</v>
       </c>
       <c r="B23" s="7" t="s">
@@ -3634,7 +3651,7 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="12" t="s">
+      <c r="A24" s="13" t="s">
         <v>41</v>
       </c>
       <c r="B24" s="7" t="s">
@@ -3651,7 +3668,7 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="12" t="s">
+      <c r="A25" s="13" t="s">
         <v>42</v>
       </c>
       <c r="B25" s="7" t="s">
@@ -3668,7 +3685,7 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="12" t="s">
+      <c r="A26" s="13" t="s">
         <v>43</v>
       </c>
       <c r="B26" s="7" t="s">
@@ -3685,7 +3702,7 @@
       </c>
     </row>
     <row r="27" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="12" t="s">
+      <c r="A27" s="13" t="s">
         <v>44</v>
       </c>
       <c r="B27" s="7" t="s">
@@ -3740,10 +3757,10 @@
         <v>47</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D30" s="7" t="n">
         <v>500</v>
@@ -3757,10 +3774,10 @@
         <v>48</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D31" s="7" t="n">
         <v>500</v>
@@ -3774,10 +3791,10 @@
         <v>49</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D32" s="7" t="n">
         <v>500</v>
@@ -3843,10 +3860,10 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Běžné"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Běžné"&amp;12Stránka &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Stránka &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>